<commit_message>
cambio a una base de datos
</commit_message>
<xml_diff>
--- a/Ayuntamiento.xlsx
+++ b/Ayuntamiento.xlsx
@@ -1,34 +1,75 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0" showHorizontalScroll="1" showVerticalScroll="1"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr fullCalcOnLoad="1"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t>Telefono</t>
+  </si>
+  <si>
+    <t>joshua</t>
+  </si>
+  <si>
+    <t>sadjlah</t>
+  </si>
+  <si>
+    <t>3294293048</t>
+  </si>
+  <si>
+    <t>alan</t>
+  </si>
+  <si>
+    <t>sajdhasj</t>
+  </si>
+  <si>
+    <t>303409099</t>
+  </si>
+  <si>
+    <t>jose</t>
+  </si>
+  <si>
+    <t>asjda</t>
+  </si>
+  <si>
+    <t>9023390429</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1">
     <font>
+      <sz val="11.000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -36,95 +77,33 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
@@ -170,13 +149,13 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Angsana New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -204,13 +183,13 @@
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Cordia New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -407,55 +386,276 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Nombre</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Apellido</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Telefono</t>
-        </is>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">joshua </t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>martinez</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>329029390</t>
-        </is>
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>